<commit_message>
Files updated Analysis written
</commit_message>
<xml_diff>
--- a/metrics_report.xlsx
+++ b/metrics_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\Coding\BoM-stylometric-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C12837-B3F0-4EDA-B812-FE7114992E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BA61CE-BB6A-4AB3-8ADC-E20173B7F5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>all</t>
   </si>
@@ -34,6 +34,9 @@
     <t>BoM&amp;D&amp;C</t>
   </si>
   <si>
+    <t>BoM&amp;D&amp;C&amp;POGP</t>
+  </si>
+  <si>
     <t>BoM&amp;POGP</t>
   </si>
   <si>
@@ -52,34 +55,40 @@
     <t>Random Forest</t>
   </si>
   <si>
-    <t>Accuracy: 0.7188
-Precision: 0.6828
-Recall: 0.7188
-F1-Score: 0.6907</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7464
-Precision: 0.6907
-Recall: 0.7464
-F1-Score: 0.7042</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.8100
-Precision: 0.7764
-Recall: 0.8100
-F1-Score: 0.7883</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.9167
-Precision: 0.9254
-Recall: 0.9167
-F1-Score: 0.9180</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.6750
-Precision: 0.6766
-Recall: 0.6750
-F1-Score: 0.6141</t>
+    <t>Accuracy: 0.7652
+Precision: 0.7796
+Recall: 0.7652
+F1-Score: 0.7488</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.8115
+Precision: 0.8204
+Recall: 0.8115
+F1-Score: 0.7979</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.8167
+Precision: 0.7814
+Recall: 0.8167
+F1-Score: 0.7941</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.9083
+Precision: 0.9164
+Recall: 0.9083
+F1-Score: 0.9097</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7400
+Precision: 0.7524
+Recall: 0.7400
+F1-Score: 0.7185</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7333
+Precision: 0.6538
+Recall: 0.7333
+F1-Score: 0.6782</t>
   </si>
   <si>
     <t>Accuracy: 0.9688
@@ -94,31 +103,31 @@
 F1-Score: 1.0000</t>
   </si>
   <si>
-    <t>Accuracy: 0.9500
-Precision: 0.9522
-Recall: 0.9500
-F1-Score: 0.9499</t>
+    <t>Accuracy: 0.9400
+Precision: 0.9434
+Recall: 0.9400
+F1-Score: 0.9398</t>
   </si>
   <si>
     <t>Accuracy: 0.8350
-Precision: 0.8387
+Precision: 0.8418
 Recall: 0.8350
-F1-Score: 0.8363</t>
+F1-Score: 0.8372</t>
   </si>
   <si>
     <t>KNN</t>
   </si>
   <si>
-    <t>Accuracy: 0.6062
-Precision: 0.5812
-Recall: 0.6062
-F1-Score: 0.5758</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7286
-Precision: 0.6673
-Recall: 0.7286
-F1-Score: 0.6802</t>
+    <t>Accuracy: 0.6696
+Precision: 0.6862
+Recall: 0.6696
+F1-Score: 0.6500</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7692
+Precision: 0.7759
+Recall: 0.7692
+F1-Score: 0.7253</t>
   </si>
   <si>
     <t>Accuracy: 0.6967
@@ -133,10 +142,16 @@
 F1-Score: 0.8919</t>
   </si>
   <si>
-    <t>Accuracy: 0.6500
-Precision: 0.5560
-Recall: 0.6500
-F1-Score: 0.5837</t>
+    <t>Accuracy: 0.7200
+Precision: 0.7354
+Recall: 0.7200
+F1-Score: 0.6940</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7222
+Precision: 0.6364
+Recall: 0.7222
+F1-Score: 0.6631</t>
   </si>
   <si>
     <t>Accuracy: 0.9062
@@ -151,12 +166,6 @@
 F1-Score: 0.9875</t>
   </si>
   <si>
-    <t>Accuracy: 0.9400
-Precision: 0.9434
-Recall: 0.9400
-F1-Score: 0.9398</t>
-  </si>
-  <si>
     <t>Accuracy: 0.7550
 Precision: 0.7609
 Recall: 0.7550
@@ -166,109 +175,115 @@
     <t>Neural Net</t>
   </si>
   <si>
-    <t>Accuracy: 0.6333
-Precision: 0.6286
-Recall: 0.6333
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.6429
-Precision: 0.6997
-Recall: 0.6429
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7433
-Precision: 0.7106
-Recall: 0.7433
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.8417
-Precision: 0.8583
-Recall: 0.8417
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.5850
-Precision: 0.6459
-Recall: 0.5850
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.8875
-Precision: 0.8884
-Recall: 0.8875
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 1.0000
-Precision: 1.0000
-Recall: 1.0000
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7900
-Precision: 0.8000
-Recall: 0.7900
-F1-Score: 0.6346</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7550
-Precision: 0.7660
-Recall: 0.7550
-F1-Score: 0.6346</t>
+    <t>Accuracy: 0.6522
+Precision: 0.6610
+Recall: 0.6522
+F1-Score: 0.6368</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.6769
+Precision: 0.6914
+Recall: 0.6769
+F1-Score: 0.6654</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7133
+Precision: 0.6899
+Recall: 0.7133
+F1-Score: 0.6950</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.8000
+Precision: 0.8147
+Recall: 0.8000
+F1-Score: 0.8040</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.6650
+Precision: 0.5659
+Recall: 0.6650
+F1-Score: 0.6013</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.6389
+Precision: 0.6347
+Recall: 0.6389
+F1-Score: 0.5980</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.8750
+Precision: 0.8717
+Recall: 0.8750
+F1-Score: 0.8718</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.8200
+Precision: 0.8344
+Recall: 0.8200
+F1-Score: 0.8205</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7600
+Precision: 0.7649
+Recall: 0.7600
+F1-Score: 0.7587</t>
   </si>
   <si>
     <t>Ensemble Model</t>
   </si>
   <si>
-    <t>Accuracy: 0.6375
-Precision: 0.6542
-Recall: 0.6375
-F1-Score: 0.6019</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.6964
-Precision: 0.7097
-Recall: 0.6964
-F1-Score: 0.6528</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7433
-Precision: 0.7322
-Recall: 0.7433
-F1-Score: 0.7183</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.8833
-Precision: 0.9062
-Recall: 0.8833
-F1-Score: 0.8851</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.6350
-Precision: 0.6522
-Recall: 0.6350
-F1-Score: 0.5820</t>
+    <t>Accuracy: 0.6848
+Precision: 0.7030
+Recall: 0.6848
+F1-Score: 0.6659</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7577
+Precision: 0.7618
+Recall: 0.7577
+F1-Score: 0.7453</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7567
+Precision: 0.7449
+Recall: 0.7567
+F1-Score: 0.7308</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.8750
+Precision: 0.8952
+Recall: 0.8750
+F1-Score: 0.8756</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.6750
+Precision: 0.6888
+Recall: 0.6750
+F1-Score: 0.6543</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.6889
+Precision: 0.6042
+Recall: 0.6889
+F1-Score: 0.6257</t>
   </si>
   <si>
     <t>Accuracy: 0.9250
-Precision: 0.9295
+Precision: 0.9305
 Recall: 0.9250
 F1-Score: 0.9235</t>
   </si>
   <si>
-    <t>Accuracy: 0.8900
-Precision: 0.8961
-Recall: 0.8900
-F1-Score: 0.8888</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.7450
-Precision: 0.7679
-Recall: 0.7450
-F1-Score: 0.7408</t>
+    <t>Accuracy: 0.8400
+Precision: 0.8597
+Recall: 0.8400
+F1-Score: 0.8287</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.7550
+Precision: 0.7771
+Recall: 0.7550
+F1-Score: 0.7463</t>
   </si>
 </sst>
 </file>
@@ -631,27 +646,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="55.21875" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" customWidth="1"/>
-    <col min="4" max="4" width="60.88671875" customWidth="1"/>
-    <col min="5" max="5" width="67" customWidth="1"/>
-    <col min="6" max="6" width="59.21875" customWidth="1"/>
-    <col min="7" max="7" width="59.5546875" customWidth="1"/>
-    <col min="8" max="8" width="63.21875" customWidth="1"/>
-    <col min="9" max="9" width="58.44140625" customWidth="1"/>
-    <col min="10" max="10" width="55.21875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="81.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,133 +682,148 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="K5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>